<commit_message>
ft: islandia fixed sol
</commit_message>
<xml_diff>
--- a/data/islandia_12.xlsx
+++ b/data/islandia_12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nico_7/Desktop/calendar-opt-master/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdduarte/Development/universidad/tesis/calendar-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD996A-E504-A340-9B06-85E27099A52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5523710-9FAC-2848-AB4F-2C6D95E5115E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -606,9 +606,6 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>22</v>
-      </c>
       <c r="B3" s="2">
         <v>44464</v>
       </c>
@@ -623,8 +620,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>22</v>
+      <c r="B4" s="2">
+        <v>44464</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -637,8 +634,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>22</v>
+      <c r="B5" s="2">
+        <v>44464</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -651,8 +648,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>22</v>
+      <c r="B6" s="2">
+        <v>44464</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -665,8 +662,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>22</v>
+      <c r="B7" s="2">
+        <v>44464</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -679,8 +676,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>22</v>
+      <c r="B8" s="2">
+        <v>44464</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -698,11 +695,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>21</v>
-      </c>
       <c r="B10" s="2">
-        <v>44458</v>
+        <v>44464</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
@@ -715,8 +709,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>21</v>
+      <c r="B11" s="2">
+        <v>44464</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -729,8 +723,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>21</v>
+      <c r="B12" s="2">
+        <v>44464</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -743,8 +737,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>21</v>
+      <c r="B13" s="2">
+        <v>44464</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -757,8 +751,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>21</v>
+      <c r="B14" s="2">
+        <v>44464</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -771,11 +765,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>21</v>
-      </c>
       <c r="B15" s="2">
-        <v>44459</v>
+        <v>44464</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -793,11 +784,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>20</v>
-      </c>
       <c r="B17" s="2">
-        <v>44450</v>
+        <v>44464</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -810,8 +798,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>20</v>
+      <c r="B18" s="2">
+        <v>44464</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -824,8 +812,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>20</v>
+      <c r="B19" s="2">
+        <v>44464</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -838,8 +826,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>20</v>
+      <c r="B20" s="2">
+        <v>44464</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -852,8 +840,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
+      <c r="B21" s="2">
+        <v>44464</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -866,11 +854,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
       <c r="B22" s="2">
-        <v>44452</v>
+        <v>44464</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -888,11 +873,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>19</v>
-      </c>
       <c r="B24" s="2">
-        <v>44436</v>
+        <v>44464</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -905,11 +887,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>19</v>
-      </c>
       <c r="B25" s="2">
-        <v>44437</v>
+        <v>44464</v>
       </c>
       <c r="C25" t="s">
         <v>16</v>
@@ -922,8 +901,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>19</v>
+      <c r="B26" s="2">
+        <v>44464</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -936,8 +915,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>19</v>
+      <c r="B27" s="2">
+        <v>44464</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -950,8 +929,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>19</v>
+      <c r="B28" s="2">
+        <v>44464</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
@@ -964,8 +943,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>19</v>
+      <c r="B29" s="2">
+        <v>44464</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -983,11 +962,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>18</v>
-      </c>
       <c r="B31" s="2">
-        <v>44429</v>
+        <v>44464</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
@@ -1000,8 +976,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>18</v>
+      <c r="B32" s="2">
+        <v>44464</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -1014,11 +990,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>18</v>
-      </c>
       <c r="B33" s="2">
-        <v>44430</v>
+        <v>44464</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1031,11 +1004,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>18</v>
-      </c>
       <c r="B34" s="2">
-        <v>44431</v>
+        <v>44464</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
@@ -1048,8 +1018,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>18</v>
+      <c r="B35" s="2">
+        <v>44464</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1062,11 +1032,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>18</v>
-      </c>
       <c r="B36" s="2">
-        <v>44433</v>
+        <v>44464</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1084,11 +1051,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>17</v>
-      </c>
       <c r="B38" s="2">
-        <v>44423</v>
+        <v>44464</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -1101,8 +1065,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>17</v>
+      <c r="B39" s="2">
+        <v>44464</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -1115,8 +1079,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>17</v>
+      <c r="B40" s="2">
+        <v>44464</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1129,11 +1093,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>17</v>
-      </c>
       <c r="B41" s="2">
-        <v>44424</v>
+        <v>44464</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -1146,8 +1107,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>17</v>
+      <c r="B42" s="2">
+        <v>44464</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -1160,8 +1121,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>17</v>
+      <c r="B43" s="2">
+        <v>44464</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1179,11 +1140,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>16</v>
-      </c>
       <c r="B45" s="2">
-        <v>44416</v>
+        <v>44464</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
@@ -1196,8 +1154,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>16</v>
+      <c r="B46" s="2">
+        <v>44464</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1210,8 +1168,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>16</v>
+      <c r="B47" s="2">
+        <v>44464</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
@@ -1224,8 +1182,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>16</v>
+      <c r="B48" s="2">
+        <v>44464</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -1238,8 +1196,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>16</v>
+      <c r="B49" s="2">
+        <v>44464</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
@@ -1252,11 +1210,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>16</v>
-      </c>
       <c r="B50" s="2">
-        <v>44417</v>
+        <v>44464</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1274,11 +1229,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>15</v>
-      </c>
       <c r="B52" s="2">
-        <v>44410</v>
+        <v>44464</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -1291,11 +1243,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>15</v>
-      </c>
       <c r="B53" s="2">
-        <v>44411</v>
+        <v>44464</v>
       </c>
       <c r="C53" t="s">
         <v>16</v>
@@ -1308,8 +1257,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>15</v>
+      <c r="B54" s="2">
+        <v>44464</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
@@ -1322,11 +1271,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>15</v>
-      </c>
       <c r="B55" s="2">
-        <v>44412</v>
+        <v>44464</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1339,8 +1285,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>15</v>
+      <c r="B56" s="2">
+        <v>44464</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1353,8 +1299,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>15</v>
+      <c r="B57" s="2">
+        <v>44464</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1372,11 +1318,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>14</v>
-      </c>
       <c r="B59" s="2">
-        <v>44402</v>
+        <v>44464</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
@@ -1389,8 +1332,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>14</v>
+      <c r="B60" s="2">
+        <v>44464</v>
       </c>
       <c r="C60" t="s">
         <v>13</v>
@@ -1403,8 +1346,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>14</v>
+      <c r="B61" s="2">
+        <v>44464</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1417,8 +1360,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>14</v>
+      <c r="B62" s="2">
+        <v>44464</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
@@ -1431,8 +1374,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>14</v>
+      <c r="B63" s="2">
+        <v>44464</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -1445,11 +1388,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>14</v>
-      </c>
       <c r="B64" s="2">
-        <v>44403</v>
+        <v>44464</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
@@ -1467,11 +1407,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>13</v>
-      </c>
       <c r="B66" s="2">
-        <v>44394</v>
+        <v>44464</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -1484,11 +1421,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>13</v>
-      </c>
       <c r="B67" s="2">
-        <v>44395</v>
+        <v>44464</v>
       </c>
       <c r="C67" t="s">
         <v>16</v>
@@ -1501,8 +1435,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>13</v>
+      <c r="B68" s="2">
+        <v>44464</v>
       </c>
       <c r="C68" t="s">
         <v>14</v>
@@ -1515,8 +1449,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>13</v>
+      <c r="B69" s="2">
+        <v>44464</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
@@ -1529,11 +1463,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>13</v>
-      </c>
       <c r="B70" s="2">
-        <v>44396</v>
+        <v>44464</v>
       </c>
       <c r="C70" t="s">
         <v>13</v>
@@ -1546,8 +1477,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>13</v>
+      <c r="B71" s="2">
+        <v>44464</v>
       </c>
       <c r="C71" t="s">
         <v>15</v>
@@ -1565,11 +1496,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>12</v>
-      </c>
       <c r="B73" s="2">
-        <v>44363</v>
+        <v>44464</v>
       </c>
       <c r="C73" t="s">
         <v>14</v>
@@ -1582,8 +1510,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>12</v>
+      <c r="B74" s="2">
+        <v>44464</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -1596,11 +1524,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>12</v>
-      </c>
       <c r="B75" s="2">
-        <v>44389</v>
+        <v>44464</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -1613,8 +1538,8 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>12</v>
+      <c r="B76" s="2">
+        <v>44464</v>
       </c>
       <c r="C76" t="s">
         <v>13</v>
@@ -1627,11 +1552,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>12</v>
-      </c>
       <c r="B77" s="2">
-        <v>44390</v>
+        <v>44464</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -1644,8 +1566,8 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>12</v>
+      <c r="B78" s="2">
+        <v>44464</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -1663,11 +1585,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>11</v>
-      </c>
       <c r="B80" s="2">
-        <v>44378</v>
+        <v>44464</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -1680,11 +1599,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>11</v>
-      </c>
       <c r="B81" s="2">
-        <v>44380</v>
+        <v>44464</v>
       </c>
       <c r="C81" t="s">
         <v>10</v>
@@ -1697,8 +1613,8 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>11</v>
+      <c r="B82" s="2">
+        <v>44464</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
@@ -1711,11 +1627,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>11</v>
-      </c>
       <c r="B83" s="2">
-        <v>44382</v>
+        <v>44464</v>
       </c>
       <c r="C83" t="s">
         <v>16</v>
@@ -1728,8 +1641,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>11</v>
+      <c r="B84" s="2">
+        <v>44464</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
@@ -1742,11 +1655,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>11</v>
-      </c>
       <c r="B85" s="2">
-        <v>44386</v>
+        <v>44464</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -1764,11 +1674,8 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>10</v>
-      </c>
       <c r="B87" s="2">
-        <v>44374</v>
+        <v>44464</v>
       </c>
       <c r="C87" t="s">
         <v>14</v>
@@ -1781,8 +1688,8 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>10</v>
+      <c r="B88" s="2">
+        <v>44464</v>
       </c>
       <c r="C88" t="s">
         <v>6</v>
@@ -1795,8 +1702,8 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>10</v>
+      <c r="B89" s="2">
+        <v>44464</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -1809,11 +1716,8 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>10</v>
-      </c>
       <c r="B90" s="2">
-        <v>44375</v>
+        <v>44464</v>
       </c>
       <c r="C90" t="s">
         <v>12</v>
@@ -1826,8 +1730,8 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>10</v>
+      <c r="B91" s="2">
+        <v>44464</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
@@ -1840,8 +1744,8 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>10</v>
+      <c r="B92" s="2">
+        <v>44464</v>
       </c>
       <c r="C92" t="s">
         <v>13</v>
@@ -1859,11 +1763,8 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>9</v>
-      </c>
       <c r="B94" s="2">
-        <v>44367</v>
+        <v>44464</v>
       </c>
       <c r="C94" t="s">
         <v>16</v>
@@ -1876,8 +1777,8 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>9</v>
+      <c r="B95" s="2">
+        <v>44464</v>
       </c>
       <c r="C95" t="s">
         <v>8</v>
@@ -1890,8 +1791,8 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>9</v>
+      <c r="B96" s="2">
+        <v>44464</v>
       </c>
       <c r="C96" t="s">
         <v>7</v>
@@ -1904,8 +1805,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>9</v>
+      <c r="B97" s="2">
+        <v>44464</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
@@ -1918,8 +1819,8 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>9</v>
+      <c r="B98" s="2">
+        <v>44464</v>
       </c>
       <c r="C98" t="s">
         <v>15</v>
@@ -1932,11 +1833,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>9</v>
-      </c>
       <c r="B99" s="2">
-        <v>44368</v>
+        <v>44464</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
@@ -1954,11 +1852,8 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>8</v>
-      </c>
       <c r="B101" s="2">
-        <v>44359</v>
+        <v>44464</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -1971,8 +1866,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>8</v>
+      <c r="B102" s="2">
+        <v>44464</v>
       </c>
       <c r="C102" t="s">
         <v>7</v>
@@ -1985,8 +1880,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>8</v>
+      <c r="B103" s="2">
+        <v>44464</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
@@ -1999,11 +1894,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>8</v>
-      </c>
       <c r="B104" s="2">
-        <v>44361</v>
+        <v>44464</v>
       </c>
       <c r="C104" t="s">
         <v>13</v>
@@ -2016,11 +1908,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>8</v>
-      </c>
       <c r="B105" s="2">
-        <v>44363</v>
+        <v>44464</v>
       </c>
       <c r="C105" t="s">
         <v>12</v>
@@ -2033,8 +1922,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>8</v>
+      <c r="B106" s="2">
+        <v>44464</v>
       </c>
       <c r="C106" t="s">
         <v>15</v>
@@ -2052,11 +1941,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>7</v>
-      </c>
       <c r="B108" s="2">
-        <v>44346</v>
+        <v>44464</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -2069,8 +1955,8 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>7</v>
+      <c r="B109" s="2">
+        <v>44464</v>
       </c>
       <c r="C109" t="s">
         <v>6</v>
@@ -2083,8 +1969,8 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>7</v>
+      <c r="B110" s="2">
+        <v>44464</v>
       </c>
       <c r="C110" t="s">
         <v>11</v>
@@ -2097,11 +1983,8 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <v>7</v>
-      </c>
       <c r="B111" s="2">
-        <v>44354</v>
+        <v>44464</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
@@ -2114,11 +1997,8 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>7</v>
-      </c>
       <c r="B112" s="2">
-        <v>44433</v>
+        <v>44464</v>
       </c>
       <c r="C112" t="s">
         <v>16</v>
@@ -2131,8 +2011,8 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113">
-        <v>7</v>
+      <c r="B113" s="2">
+        <v>44464</v>
       </c>
       <c r="C113" t="s">
         <v>14</v>
@@ -2150,11 +2030,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115">
-        <v>6</v>
-      </c>
       <c r="B115" s="2">
-        <v>44340</v>
+        <v>44464</v>
       </c>
       <c r="C115" t="s">
         <v>15</v>
@@ -2167,8 +2044,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>6</v>
+      <c r="B116" s="2">
+        <v>44464</v>
       </c>
       <c r="C116" t="s">
         <v>7</v>
@@ -2181,8 +2058,8 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117">
-        <v>6</v>
+      <c r="B117" s="2">
+        <v>44464</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
@@ -2195,11 +2072,8 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118">
-        <v>6</v>
-      </c>
       <c r="B118" s="2">
-        <v>44341</v>
+        <v>44464</v>
       </c>
       <c r="C118" t="s">
         <v>13</v>
@@ -2212,8 +2086,8 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119">
-        <v>6</v>
+      <c r="B119" s="2">
+        <v>44464</v>
       </c>
       <c r="C119" t="s">
         <v>11</v>
@@ -2226,8 +2100,8 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120">
-        <v>6</v>
+      <c r="B120" s="2">
+        <v>44464</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
@@ -2245,11 +2119,8 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122">
-        <v>5</v>
-      </c>
       <c r="B122" s="2">
-        <v>44337</v>
+        <v>44464</v>
       </c>
       <c r="C122" t="s">
         <v>16</v>
@@ -2262,8 +2133,8 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123">
-        <v>5</v>
+      <c r="B123" s="2">
+        <v>44464</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
@@ -2276,8 +2147,8 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124">
-        <v>5</v>
+      <c r="B124" s="2">
+        <v>44464</v>
       </c>
       <c r="C124" t="s">
         <v>10</v>
@@ -2290,8 +2161,8 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125">
-        <v>5</v>
+      <c r="B125" s="2">
+        <v>44464</v>
       </c>
       <c r="C125" t="s">
         <v>8</v>
@@ -2304,8 +2175,8 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126">
-        <v>5</v>
+      <c r="B126" s="2">
+        <v>44464</v>
       </c>
       <c r="C126" t="s">
         <v>5</v>
@@ -2318,11 +2189,8 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127">
-        <v>5</v>
-      </c>
       <c r="B127" s="2">
-        <v>44338</v>
+        <v>44464</v>
       </c>
       <c r="C127" t="s">
         <v>14</v>
@@ -2340,11 +2208,8 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129">
-        <v>4</v>
-      </c>
       <c r="B129" s="2">
-        <v>44332</v>
+        <v>44464</v>
       </c>
       <c r="C129" t="s">
         <v>13</v>
@@ -2357,8 +2222,8 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130">
-        <v>4</v>
+      <c r="B130" s="2">
+        <v>44464</v>
       </c>
       <c r="C130" t="s">
         <v>9</v>
@@ -2371,11 +2236,8 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131">
-        <v>4</v>
-      </c>
       <c r="B131" s="2">
-        <v>44333</v>
+        <v>44464</v>
       </c>
       <c r="C131" t="s">
         <v>15</v>
@@ -2388,8 +2250,8 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132">
-        <v>4</v>
+      <c r="B132" s="2">
+        <v>44464</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
@@ -2402,8 +2264,8 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133">
-        <v>4</v>
+      <c r="B133" s="2">
+        <v>44464</v>
       </c>
       <c r="C133" t="s">
         <v>11</v>
@@ -2416,8 +2278,8 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134">
-        <v>4</v>
+      <c r="B134" s="2">
+        <v>44464</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
@@ -2435,11 +2297,8 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136">
-        <v>3</v>
-      </c>
       <c r="B136" s="2">
-        <v>44328</v>
+        <v>44464</v>
       </c>
       <c r="C136" t="s">
         <v>16</v>
@@ -2452,8 +2311,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137">
-        <v>3</v>
+      <c r="B137" s="2">
+        <v>44464</v>
       </c>
       <c r="C137" t="s">
         <v>8</v>
@@ -2466,11 +2325,8 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138">
-        <v>3</v>
-      </c>
       <c r="B138" s="2">
-        <v>44329</v>
+        <v>44464</v>
       </c>
       <c r="C138" t="s">
         <v>5</v>
@@ -2483,8 +2339,8 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139">
-        <v>3</v>
+      <c r="B139" s="2">
+        <v>44464</v>
       </c>
       <c r="C139" t="s">
         <v>14</v>
@@ -2497,8 +2353,8 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140">
-        <v>3</v>
+      <c r="B140" s="2">
+        <v>44464</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -2511,8 +2367,8 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141">
-        <v>3</v>
+      <c r="B141" s="2">
+        <v>44464</v>
       </c>
       <c r="C141" t="s">
         <v>10</v>
@@ -2530,11 +2386,8 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143">
-        <v>2</v>
-      </c>
       <c r="B143" s="2">
-        <v>44323</v>
+        <v>44464</v>
       </c>
       <c r="C143" t="s">
         <v>11</v>
@@ -2547,11 +2400,8 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144">
-        <v>2</v>
-      </c>
       <c r="B144" s="2">
-        <v>44324</v>
+        <v>44464</v>
       </c>
       <c r="C144" t="s">
         <v>12</v>
@@ -2564,8 +2414,8 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145">
-        <v>2</v>
+      <c r="B145" s="2">
+        <v>44464</v>
       </c>
       <c r="C145" t="s">
         <v>13</v>
@@ -2578,8 +2428,8 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146">
-        <v>2</v>
+      <c r="B146" s="2">
+        <v>44464</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -2592,11 +2442,8 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147">
-        <v>2</v>
-      </c>
       <c r="B147" s="2">
-        <v>44325</v>
+        <v>44464</v>
       </c>
       <c r="C147" t="s">
         <v>14</v>
@@ -2609,8 +2456,8 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148">
-        <v>2</v>
+      <c r="B148" s="2">
+        <v>44464</v>
       </c>
       <c r="C148" t="s">
         <v>15</v>
@@ -2628,11 +2475,8 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150">
-        <v>1</v>
-      </c>
       <c r="B150" s="2">
-        <v>44316</v>
+        <v>44464</v>
       </c>
       <c r="C150" t="s">
         <v>5</v>
@@ -2645,11 +2489,8 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151">
-        <v>1</v>
-      </c>
       <c r="B151" s="2">
-        <v>44317</v>
+        <v>44464</v>
       </c>
       <c r="C151" t="s">
         <v>6</v>
@@ -2662,8 +2503,8 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152">
-        <v>1</v>
+      <c r="B152" s="2">
+        <v>44464</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
@@ -2676,8 +2517,8 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153">
-        <v>1</v>
+      <c r="B153" s="2">
+        <v>44464</v>
       </c>
       <c r="C153" t="s">
         <v>8</v>
@@ -2690,11 +2531,8 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154">
-        <v>1</v>
-      </c>
       <c r="B154" s="2">
-        <v>44318</v>
+        <v>44464</v>
       </c>
       <c r="C154" t="s">
         <v>9</v>
@@ -2707,8 +2545,8 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155">
-        <v>1</v>
+      <c r="B155" s="2">
+        <v>44464</v>
       </c>
       <c r="C155" t="s">
         <v>10</v>

</xml_diff>